<commit_message>
Updated some values in Excel spreadsheet following review of existing Persistent Volumes in k8s
</commit_message>
<xml_diff>
--- a/documentation/SKY-ElasticSearch-Cluster-Kubernetes-Dev-Env.xlsx
+++ b/documentation/SKY-ElasticSearch-Cluster-Kubernetes-Dev-Env.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevejones/Dropbox/WebturaLTD/Clients/DellEMC/SKY-ES-Dev-Upgrade-Plan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevejones/Projects/DellEMC-Sky/k8s/smj-kubeapps/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE042C7-F7B8-F442-821D-72BFA91B4167}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D3AF31-08C2-8F4C-BF05-16DF8295E2A6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="26860" windowHeight="18000" xr2:uid="{E1CBD3F7-F122-8243-AA37-C7A12BB3D86F}"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="29700" windowHeight="18520" activeTab="1" xr2:uid="{E1CBD3F7-F122-8243-AA37-C7A12BB3D86F}"/>
   </bookViews>
   <sheets>
     <sheet name="Node Specs" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="51">
   <si>
     <t>Node Type</t>
   </si>
@@ -179,12 +179,21 @@
   </si>
   <si>
     <t>ElasticSearch Cluster Environment (sky_elastic_01)</t>
+  </si>
+  <si>
+    <t>Total Used (TB)</t>
+  </si>
+  <si>
+    <t>Percentage Used</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -304,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -339,6 +348,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -346,6 +356,27 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB76C48-6AC6-CE46-8248-44E0423F649C}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -681,13 +712,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
@@ -747,15 +778,15 @@
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -995,16 +1026,16 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1259,14 +1290,14 @@
     <row r="31" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:9" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
@@ -1320,34 +1351,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9C241A-089D-FF47-B54B-0A887D0714B1}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.5" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="9"/>
+    <col min="8" max="8" width="7.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="9"/>
+    <col min="10" max="10" width="25" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="17" width="18.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-    </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+    </row>
+    <row r="2" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
@@ -1373,8 +1408,33 @@
         <f>SUM(B3:G3)</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="24">
+        <v>11</v>
+      </c>
+      <c r="L3" s="24">
+        <v>11</v>
+      </c>
+      <c r="M3" s="24">
+        <v>11</v>
+      </c>
+      <c r="N3" s="24">
+        <v>11</v>
+      </c>
+      <c r="O3" s="24">
+        <v>11</v>
+      </c>
+      <c r="P3" s="24">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="25">
+        <f>SUM(K3:P3)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>24</v>
       </c>
@@ -1396,8 +1456,30 @@
       <c r="G4" s="10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="20"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
@@ -1407,8 +1489,18 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="27"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1420,8 +1512,18 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="28"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="27"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>27</v>
       </c>
@@ -1431,8 +1533,18 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="27"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>28</v>
       </c>
@@ -1442,8 +1554,18 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="27"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>29</v>
       </c>
@@ -1465,8 +1587,30 @@
       <c r="G9" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="29">
+        <v>0</v>
+      </c>
+      <c r="L9" s="29">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="M9" s="29">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="N9" s="30">
+        <v>0</v>
+      </c>
+      <c r="O9" s="29">
+        <v>0.106</v>
+      </c>
+      <c r="P9" s="29">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="Q9" s="27"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>30</v>
       </c>
@@ -1488,8 +1632,30 @@
       <c r="G10" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="29">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="L10" s="29">
+        <v>0</v>
+      </c>
+      <c r="M10" s="29">
+        <v>0</v>
+      </c>
+      <c r="N10" s="29">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="O10" s="30">
+        <v>0</v>
+      </c>
+      <c r="P10" s="29">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="Q10" s="27"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>31</v>
       </c>
@@ -1511,8 +1677,30 @@
       <c r="G11" s="15">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="29">
+        <v>0.505</v>
+      </c>
+      <c r="L11" s="29">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="M11" s="29">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="N11" s="29">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="O11" s="29">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="P11" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="27"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>32</v>
       </c>
@@ -1522,8 +1710,18 @@
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="27"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>33</v>
       </c>
@@ -1533,8 +1731,18 @@
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="27"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>34</v>
       </c>
@@ -1544,8 +1752,18 @@
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="27"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>35</v>
       </c>
@@ -1555,8 +1773,18 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="27"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>36</v>
       </c>
@@ -1566,8 +1794,18 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J16" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="27"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>37</v>
       </c>
@@ -1577,8 +1815,18 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="27"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>38</v>
       </c>
@@ -1588,8 +1836,18 @@
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J18" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="27"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>39</v>
       </c>
@@ -1599,8 +1857,18 @@
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J19" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="27"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>40</v>
       </c>
@@ -1610,8 +1878,18 @@
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J20" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="27"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>41</v>
       </c>
@@ -1621,8 +1899,18 @@
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="27"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>42</v>
       </c>
@@ -1632,8 +1920,18 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J22" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="27"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>43</v>
       </c>
@@ -1643,8 +1941,18 @@
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J23" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+      <c r="Q23" s="27"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>44</v>
       </c>
@@ -1654,8 +1962,18 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="27"/>
+    </row>
+    <row r="25" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>47</v>
       </c>
@@ -1687,8 +2005,39 @@
         <f>SUM(B25:G25)</f>
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="K25" s="31">
+        <f>SUM(K5:K24)</f>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="L25" s="31">
+        <f t="shared" ref="L25:P25" si="1">SUM(L5:L24)</f>
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="M25" s="31">
+        <f t="shared" si="1"/>
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="N25" s="31">
+        <f t="shared" si="1"/>
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="O25" s="31">
+        <f t="shared" si="1"/>
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="P25" s="31">
+        <f t="shared" si="1"/>
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="Q25" s="32">
+        <f>SUM(K25:P25)</f>
+        <v>4.8860000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>46</v>
       </c>
@@ -1697,28 +2046,92 @@
         <v>7.9</v>
       </c>
       <c r="C26" s="16">
-        <f t="shared" ref="C26:H26" si="1">C3-C25</f>
+        <f t="shared" ref="C26:H26" si="2">C3-C25</f>
         <v>8</v>
       </c>
       <c r="D26" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="E26" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="F26" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G26" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="H26" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47.9</v>
+      </c>
+      <c r="J26" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="31">
+        <f>K3-K25</f>
+        <v>10.024000000000001</v>
+      </c>
+      <c r="L26" s="31">
+        <f t="shared" ref="L26:Q26" si="3">L3-L25</f>
+        <v>10.057</v>
+      </c>
+      <c r="M26" s="31">
+        <f t="shared" si="3"/>
+        <v>10.363</v>
+      </c>
+      <c r="N26" s="31">
+        <f t="shared" si="3"/>
+        <v>10.196999999999999</v>
+      </c>
+      <c r="O26" s="31">
+        <f t="shared" si="3"/>
+        <v>10.417</v>
+      </c>
+      <c r="P26" s="31">
+        <f t="shared" si="3"/>
+        <v>10.056000000000001</v>
+      </c>
+      <c r="Q26" s="31">
+        <f t="shared" si="3"/>
+        <v>61.113999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J27" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="9">
+        <f>K25/B25*100</f>
+        <v>31.483870967741932</v>
+      </c>
+      <c r="L27" s="9">
+        <f t="shared" ref="L27:Q27" si="4">L25/C25*100</f>
+        <v>31.43333333333333</v>
+      </c>
+      <c r="M27" s="9">
+        <f t="shared" si="4"/>
+        <v>21.233333333333334</v>
+      </c>
+      <c r="N27" s="9">
+        <f t="shared" si="4"/>
+        <v>26.766666666666666</v>
+      </c>
+      <c r="O27" s="9">
+        <f t="shared" si="4"/>
+        <v>19.433333333333334</v>
+      </c>
+      <c r="P27" s="9">
+        <f t="shared" si="4"/>
+        <v>31.466666666666665</v>
+      </c>
+      <c r="Q27" s="9">
+        <f t="shared" si="4"/>
+        <v>26.994475138121544</v>
       </c>
     </row>
   </sheetData>
@@ -1745,17 +2158,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added updates to Excel doc
</commit_message>
<xml_diff>
--- a/documentation/SKY-ElasticSearch-Cluster-Kubernetes-Dev-Env.xlsx
+++ b/documentation/SKY-ElasticSearch-Cluster-Kubernetes-Dev-Env.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevejones/Projects/DellEMC-Sky/k8s/smj-kubeapps/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F7C9F7-2575-394E-950B-C166DC6E996E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC6B02F-B13F-7344-A727-DB62654F6B2A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="29700" windowHeight="18520" xr2:uid="{E1CBD3F7-F122-8243-AA37-C7A12BB3D86F}"/>
+    <workbookView xWindow="8680" yWindow="460" windowWidth="29700" windowHeight="18520" activeTab="2" xr2:uid="{E1CBD3F7-F122-8243-AA37-C7A12BB3D86F}"/>
   </bookViews>
   <sheets>
     <sheet name="Node Specs" sheetId="1" r:id="rId1"/>
     <sheet name="Existing PVs" sheetId="3" r:id="rId2"/>
     <sheet name="Proposed PVs" sheetId="4" r:id="rId3"/>
+    <sheet name="PV Allocations" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="83">
   <si>
     <t>Node Type</t>
   </si>
@@ -185,6 +186,102 @@
   </si>
   <si>
     <t>Percentage Used</t>
+  </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>master-0</t>
+  </si>
+  <si>
+    <t>master-1</t>
+  </si>
+  <si>
+    <t>master-2</t>
+  </si>
+  <si>
+    <t>data-0</t>
+  </si>
+  <si>
+    <t>data-1</t>
+  </si>
+  <si>
+    <t>data-2</t>
+  </si>
+  <si>
+    <t>data-3</t>
+  </si>
+  <si>
+    <t>data-4</t>
+  </si>
+  <si>
+    <t>data-5</t>
+  </si>
+  <si>
+    <t>data-6</t>
+  </si>
+  <si>
+    <t>data-7</t>
+  </si>
+  <si>
+    <t>data-8</t>
+  </si>
+  <si>
+    <t>data-9</t>
+  </si>
+  <si>
+    <t>data-10</t>
+  </si>
+  <si>
+    <t>data-11</t>
+  </si>
+  <si>
+    <t>Persistent Volume</t>
+  </si>
+  <si>
+    <t>es2-vol6</t>
+  </si>
+  <si>
+    <t>es1-vol5</t>
+  </si>
+  <si>
+    <t>es3-vol6</t>
+  </si>
+  <si>
+    <t>es3-vol7</t>
+  </si>
+  <si>
+    <t>es7-vol6</t>
+  </si>
+  <si>
+    <t>es1-vol6</t>
+  </si>
+  <si>
+    <t>es6-vol5</t>
+  </si>
+  <si>
+    <t>es5-vol7</t>
+  </si>
+  <si>
+    <t>es2-vol7</t>
+  </si>
+  <si>
+    <t>es6-vol7</t>
+  </si>
+  <si>
+    <t>es1-vol7</t>
+  </si>
+  <si>
+    <t>es7-vol5</t>
+  </si>
+  <si>
+    <t>es2-vol5</t>
+  </si>
+  <si>
+    <t>es5-vol6</t>
+  </si>
+  <si>
+    <t>es3-vol5</t>
   </si>
 </sst>
 </file>
@@ -349,13 +446,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -377,6 +467,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB76C48-6AC6-CE46-8248-44E0423F649C}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -712,13 +809,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
@@ -778,15 +875,15 @@
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1026,16 +1123,16 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1290,14 +1387,14 @@
     <row r="31" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:9" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
     </row>
     <row r="34" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
@@ -1354,7 +1451,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:Q27"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1369,17 +1466,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1411,25 +1508,25 @@
       <c r="J3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="24">
+      <c r="K3" s="21">
         <v>11</v>
       </c>
-      <c r="L3" s="24">
+      <c r="L3" s="21">
         <v>11</v>
       </c>
-      <c r="M3" s="24">
+      <c r="M3" s="21">
         <v>11</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="21">
         <v>11</v>
       </c>
-      <c r="O3" s="24">
+      <c r="O3" s="21">
         <v>11</v>
       </c>
-      <c r="P3" s="24">
+      <c r="P3" s="21">
         <v>11</v>
       </c>
-      <c r="Q3" s="25">
+      <c r="Q3" s="22">
         <f>SUM(K3:P3)</f>
         <v>66</v>
       </c>
@@ -1492,13 +1589,13 @@
       <c r="J5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="27"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -1515,13 +1612,13 @@
       <c r="J6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="K6" s="28"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="27"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="24"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -1536,13 +1633,13 @@
       <c r="J7" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="27"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="24"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -1557,13 +1654,13 @@
       <c r="J8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="27"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="24"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
@@ -1590,25 +1687,25 @@
       <c r="J9" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="29">
+      <c r="K9" s="26">
         <v>0</v>
       </c>
-      <c r="L9" s="29">
+      <c r="L9" s="26">
         <v>0.47099999999999997</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M9" s="26">
         <v>0.47099999999999997</v>
       </c>
-      <c r="N9" s="30">
+      <c r="N9" s="27">
         <v>0</v>
       </c>
-      <c r="O9" s="29">
+      <c r="O9" s="26">
         <v>0.106</v>
       </c>
-      <c r="P9" s="29">
+      <c r="P9" s="26">
         <v>0.47199999999999998</v>
       </c>
-      <c r="Q9" s="27"/>
+      <c r="Q9" s="24"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -1635,25 +1732,25 @@
       <c r="J10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="26">
         <v>0.47099999999999997</v>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="26">
         <v>0</v>
       </c>
-      <c r="M10" s="29">
+      <c r="M10" s="26">
         <v>0</v>
       </c>
-      <c r="N10" s="29">
+      <c r="N10" s="26">
         <v>0.40200000000000002</v>
       </c>
-      <c r="O10" s="30">
+      <c r="O10" s="27">
         <v>0</v>
       </c>
-      <c r="P10" s="29">
+      <c r="P10" s="26">
         <v>0.47199999999999998</v>
       </c>
-      <c r="Q10" s="27"/>
+      <c r="Q10" s="24"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
@@ -1680,25 +1777,25 @@
       <c r="J11" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="29">
+      <c r="K11" s="26">
         <v>0.505</v>
       </c>
-      <c r="L11" s="29">
+      <c r="L11" s="26">
         <v>0.47199999999999998</v>
       </c>
-      <c r="M11" s="29">
+      <c r="M11" s="26">
         <v>0.16600000000000001</v>
       </c>
-      <c r="N11" s="29">
+      <c r="N11" s="26">
         <v>0.40100000000000002</v>
       </c>
-      <c r="O11" s="29">
+      <c r="O11" s="26">
         <v>0.47699999999999998</v>
       </c>
-      <c r="P11" s="30">
+      <c r="P11" s="27">
         <v>0</v>
       </c>
-      <c r="Q11" s="27"/>
+      <c r="Q11" s="24"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
@@ -1713,13 +1810,13 @@
       <c r="J12" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="27"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="24"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
@@ -1734,13 +1831,13 @@
       <c r="J13" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="27"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="24"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -1755,13 +1852,13 @@
       <c r="J14" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="27"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="24"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
@@ -1776,13 +1873,13 @@
       <c r="J15" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="27"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="24"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -1797,13 +1894,13 @@
       <c r="J16" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="27"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="24"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
@@ -1818,13 +1915,13 @@
       <c r="J17" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="27"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="24"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
@@ -1839,13 +1936,13 @@
       <c r="J18" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="27"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="24"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
@@ -1860,13 +1957,13 @@
       <c r="J19" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="27"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="24"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -1881,13 +1978,13 @@
       <c r="J20" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="27"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="24"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
@@ -1902,13 +1999,13 @@
       <c r="J21" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="27"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="24"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
@@ -1923,13 +2020,13 @@
       <c r="J22" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="27"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="24"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
@@ -1944,13 +2041,13 @@
       <c r="J23" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="27"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="24"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
@@ -1965,13 +2062,13 @@
       <c r="J24" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="27"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="24"/>
     </row>
     <row r="25" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
@@ -2008,31 +2105,31 @@
       <c r="J25" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="K25" s="31">
+      <c r="K25" s="28">
         <f>SUM(K5:K24)</f>
         <v>0.97599999999999998</v>
       </c>
-      <c r="L25" s="31">
+      <c r="L25" s="28">
         <f t="shared" ref="L25:P25" si="1">SUM(L5:L24)</f>
         <v>0.94299999999999995</v>
       </c>
-      <c r="M25" s="31">
+      <c r="M25" s="28">
         <f t="shared" si="1"/>
         <v>0.63700000000000001</v>
       </c>
-      <c r="N25" s="31">
+      <c r="N25" s="28">
         <f t="shared" si="1"/>
         <v>0.80300000000000005</v>
       </c>
-      <c r="O25" s="31">
+      <c r="O25" s="28">
         <f t="shared" si="1"/>
         <v>0.58299999999999996</v>
       </c>
-      <c r="P25" s="31">
+      <c r="P25" s="28">
         <f t="shared" si="1"/>
         <v>0.94399999999999995</v>
       </c>
-      <c r="Q25" s="32">
+      <c r="Q25" s="29">
         <f>SUM(K25:P25)</f>
         <v>4.8860000000000001</v>
       </c>
@@ -2072,31 +2169,31 @@
       <c r="J26" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="K26" s="31">
+      <c r="K26" s="28">
         <f>K3-K25</f>
         <v>10.024000000000001</v>
       </c>
-      <c r="L26" s="31">
+      <c r="L26" s="28">
         <f t="shared" ref="L26:Q26" si="3">L3-L25</f>
         <v>10.057</v>
       </c>
-      <c r="M26" s="31">
+      <c r="M26" s="28">
         <f t="shared" si="3"/>
         <v>10.363</v>
       </c>
-      <c r="N26" s="31">
+      <c r="N26" s="28">
         <f t="shared" si="3"/>
         <v>10.196999999999999</v>
       </c>
-      <c r="O26" s="31">
+      <c r="O26" s="28">
         <f t="shared" si="3"/>
         <v>10.417</v>
       </c>
-      <c r="P26" s="31">
+      <c r="P26" s="28">
         <f t="shared" si="3"/>
         <v>10.056000000000001</v>
       </c>
-      <c r="Q26" s="31">
+      <c r="Q26" s="28">
         <f t="shared" si="3"/>
         <v>61.113999999999997</v>
       </c>
@@ -2105,31 +2202,31 @@
       <c r="J27" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K27" s="27">
+      <c r="K27" s="24">
         <f>K25/B25*100</f>
         <v>31.483870967741932</v>
       </c>
-      <c r="L27" s="27">
+      <c r="L27" s="24">
         <f t="shared" ref="L27:Q27" si="4">L25/C25*100</f>
         <v>31.43333333333333</v>
       </c>
-      <c r="M27" s="27">
+      <c r="M27" s="24">
         <f t="shared" si="4"/>
         <v>21.233333333333334</v>
       </c>
-      <c r="N27" s="27">
+      <c r="N27" s="24">
         <f t="shared" si="4"/>
         <v>26.766666666666666</v>
       </c>
-      <c r="O27" s="27">
+      <c r="O27" s="24">
         <f t="shared" si="4"/>
         <v>19.433333333333334</v>
       </c>
-      <c r="P27" s="27">
+      <c r="P27" s="24">
         <f t="shared" si="4"/>
         <v>31.466666666666665</v>
       </c>
-      <c r="Q27" s="27">
+      <c r="Q27" s="24">
         <f t="shared" si="4"/>
         <v>26.994475138121544</v>
       </c>
@@ -2146,7 +2243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7421E8F-D2FF-5E47-9359-2F06416A8EDC}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -2158,17 +2255,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -2588,4 +2685,201 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C5AA977-F9DE-C34A-B98B-23B89E29D345}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Proposed re-RAID of disks to build 20x3Tb data nodes with raw disks
</commit_message>
<xml_diff>
--- a/documentation/SKY-ElasticSearch-Cluster-Kubernetes-Dev-Env.xlsx
+++ b/documentation/SKY-ElasticSearch-Cluster-Kubernetes-Dev-Env.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevejones/Projects/DellEMC-Sky/k8s/smj-kubeapps/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC6B02F-B13F-7344-A727-DB62654F6B2A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8C2298-9421-CC41-B0C5-EC1250E10A13}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8680" yWindow="460" windowWidth="29700" windowHeight="18520" activeTab="2" xr2:uid="{E1CBD3F7-F122-8243-AA37-C7A12BB3D86F}"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="29700" windowHeight="18520" activeTab="4" xr2:uid="{E1CBD3F7-F122-8243-AA37-C7A12BB3D86F}"/>
   </bookViews>
   <sheets>
     <sheet name="Node Specs" sheetId="1" r:id="rId1"/>
     <sheet name="Existing PVs" sheetId="3" r:id="rId2"/>
     <sheet name="Proposed PVs" sheetId="4" r:id="rId3"/>
     <sheet name="PV Allocations" sheetId="5" r:id="rId4"/>
+    <sheet name="Proposed PVs (NoRaid - Raw)" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="83">
   <si>
     <t>Node Type</t>
   </si>
@@ -410,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -467,6 +468,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -809,13 +811,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" s="6" customFormat="1" ht="26" x14ac:dyDescent="0.3">
@@ -875,15 +877,15 @@
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1123,16 +1125,16 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1387,14 +1389,14 @@
     <row r="31" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:9" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
     </row>
     <row r="34" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
@@ -1466,17 +1468,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -2243,8 +2245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7421E8F-D2FF-5E47-9359-2F06416A8EDC}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -2255,17 +2257,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -2882,4 +2884,254 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59882CDC-BA93-0E45-9265-F250206DA38F}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+    </row>
+    <row r="2" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="11">
+        <v>14</v>
+      </c>
+      <c r="C3" s="11">
+        <v>14</v>
+      </c>
+      <c r="D3" s="11">
+        <v>14</v>
+      </c>
+      <c r="E3" s="11">
+        <v>14</v>
+      </c>
+      <c r="F3" s="11">
+        <v>14</v>
+      </c>
+      <c r="G3" s="11">
+        <v>14</v>
+      </c>
+      <c r="H3" s="16">
+        <f>SUM(B3:G3)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14">
+        <v>3</v>
+      </c>
+      <c r="D5" s="14">
+        <v>3</v>
+      </c>
+      <c r="E5" s="14">
+        <v>3</v>
+      </c>
+      <c r="F5" s="14">
+        <v>3</v>
+      </c>
+      <c r="G5" s="14">
+        <v>3</v>
+      </c>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="14">
+        <v>3</v>
+      </c>
+      <c r="C6" s="14">
+        <v>3</v>
+      </c>
+      <c r="D6" s="14">
+        <v>3</v>
+      </c>
+      <c r="E6" s="14">
+        <v>3</v>
+      </c>
+      <c r="F6" s="14">
+        <v>3</v>
+      </c>
+      <c r="G6" s="14">
+        <v>3</v>
+      </c>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="14">
+        <v>3</v>
+      </c>
+      <c r="C7" s="14">
+        <v>3</v>
+      </c>
+      <c r="D7" s="14">
+        <v>3</v>
+      </c>
+      <c r="E7" s="14">
+        <v>3</v>
+      </c>
+      <c r="F7" s="14">
+        <v>3</v>
+      </c>
+      <c r="G7" s="14">
+        <v>3</v>
+      </c>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="14">
+        <v>3</v>
+      </c>
+      <c r="C8" s="14">
+        <v>3</v>
+      </c>
+      <c r="D8" s="14">
+        <v>3</v>
+      </c>
+      <c r="E8" s="14">
+        <v>3</v>
+      </c>
+      <c r="F8" s="14">
+        <v>3</v>
+      </c>
+      <c r="G8" s="14">
+        <v>3</v>
+      </c>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="16">
+        <f>SUM(B5:B8)</f>
+        <v>12</v>
+      </c>
+      <c r="C9" s="16">
+        <f>SUM(C5:C8)</f>
+        <v>12</v>
+      </c>
+      <c r="D9" s="16">
+        <f>SUM(D5:D8)</f>
+        <v>12</v>
+      </c>
+      <c r="E9" s="16">
+        <f>SUM(E5:E8)</f>
+        <v>12</v>
+      </c>
+      <c r="F9" s="16">
+        <f>SUM(F5:F8)</f>
+        <v>12</v>
+      </c>
+      <c r="G9" s="16">
+        <f>SUM(G5:G8)</f>
+        <v>12</v>
+      </c>
+      <c r="H9" s="16">
+        <f>SUM(B9:G9)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="16">
+        <f>B3-B9</f>
+        <v>2</v>
+      </c>
+      <c r="C10" s="16">
+        <f>C3-C9</f>
+        <v>2</v>
+      </c>
+      <c r="D10" s="16">
+        <f>D3-D9</f>
+        <v>2</v>
+      </c>
+      <c r="E10" s="16">
+        <f>E3-E9</f>
+        <v>2</v>
+      </c>
+      <c r="F10" s="16">
+        <f>F3-F9</f>
+        <v>2</v>
+      </c>
+      <c r="G10" s="16">
+        <f>G3-G9</f>
+        <v>2</v>
+      </c>
+      <c r="H10" s="16">
+        <f>H3-H9</f>
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>